<commit_message>
fixed god name and finished most of the god abilites
</commit_message>
<xml_diff>
--- a/God-Abilities.xlsx
+++ b/God-Abilities.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Neumont\CSC150\Gods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neumont-my.sharepoint.com/personal/jborda_student_neumont_edu/Documents/Intro to CS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" xr2:uid="{1A2FBC8E-7367-445F-AFE7-76DC3F6C7797}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9036" windowHeight="6060" xr2:uid="{1A2FBC8E-7367-445F-AFE7-76DC3F6C7797}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>NEUMONT</t>
   </si>
@@ -59,15 +59,9 @@
     <t>MESSENGER</t>
   </si>
   <si>
-    <t>Posieden</t>
-  </si>
-  <si>
     <t>Aegir: Party: Puts random opponent creatures to sleep</t>
   </si>
   <si>
-    <t>Neptune</t>
-  </si>
-  <si>
     <t>Veruna</t>
   </si>
   <si>
@@ -95,24 +89,15 @@
     <t>Freya: Distraction: Both players lose a turn.</t>
   </si>
   <si>
-    <t>Venus</t>
-  </si>
-  <si>
     <t>Rati</t>
   </si>
   <si>
     <t>Self-sacrifice: -1 health to player +1 to all creatures</t>
   </si>
   <si>
-    <t>Zeus</t>
-  </si>
-  <si>
     <t>Odin: Mutiny: Random opponent creature attacks owner</t>
   </si>
   <si>
-    <t>Jupiter</t>
-  </si>
-  <si>
     <t>Indra</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>Hel: Necromancy: 1 creature comes back from dead with 1/2 damage</t>
   </si>
   <si>
-    <t>Pluto</t>
-  </si>
-  <si>
     <t>Yama</t>
   </si>
   <si>
@@ -147,6 +129,27 @@
   </si>
   <si>
     <t>Mercury: Regenerates random amount of mana</t>
+  </si>
+  <si>
+    <t>Zeus: draw a card from opponents hand and play it</t>
+  </si>
+  <si>
+    <t>Posiedon: Opponents God ability cannot be used</t>
+  </si>
+  <si>
+    <t>Neptune: put opponents creatures to sleep that matches your creatures</t>
+  </si>
+  <si>
+    <t>Venus: One card goes back to your hand if it "dies"</t>
+  </si>
+  <si>
+    <t>Copy opponents card</t>
+  </si>
+  <si>
+    <t>Pluto: One card from opponents discard goes to your hand</t>
+  </si>
+  <si>
+    <t>Jupiter: Opponents hand gets shuffled and they can't see any of their cards</t>
   </si>
 </sst>
 </file>
@@ -498,23 +501,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB60372-CB74-46BA-A68B-A466051590B7}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M165" sqref="M165"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.47265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.89453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="79.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -531,123 +534,128 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished adding in the hindu gods abilities
</commit_message>
<xml_diff>
--- a/God-Abilities.xlsx
+++ b/God-Abilities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paige\eclipse-workspace\CSC150\Reposity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica Borda\eclipse-workspace\tcg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,9 +62,6 @@
     <t>Aegir: Party: Puts random opponent creatures to sleep</t>
   </si>
   <si>
-    <t>Veruna</t>
-  </si>
-  <si>
     <t>Story Time: Copies opponent ability</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Mars: Raze: All creatures attack next turn for opponent</t>
   </si>
   <si>
-    <t>Karttikeyn</t>
-  </si>
-  <si>
     <t>Grows Beard: 2x damage 1 turn</t>
   </si>
   <si>
@@ -89,18 +83,12 @@
     <t>Freya: Distraction: Both players lose a turn.</t>
   </si>
   <si>
-    <t>Rati</t>
-  </si>
-  <si>
     <t>Self-sacrifice: -1 health to player +1 to all creatures</t>
   </si>
   <si>
     <t>Odin: Mutiny: Random opponent creature attacks owner</t>
   </si>
   <si>
-    <t>Indra</t>
-  </si>
-  <si>
     <t>Krebsinator: Randomly picks an opponents card from deck and plays it instantly on your battlefield</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>Hel: Necromancy: 1 creature comes back from dead with 1/2 damage</t>
   </si>
   <si>
-    <t>Yama</t>
-  </si>
-  <si>
     <t>Ramble: Bring back all packet tracer cards from discard</t>
   </si>
   <si>
@@ -122,9 +107,6 @@
     <t>Hermod: Double damage for 2 or 1 damage creatures</t>
   </si>
   <si>
-    <t>Asni</t>
-  </si>
-  <si>
     <t>Take on too much: Double mana</t>
   </si>
   <si>
@@ -147,6 +129,24 @@
   </si>
   <si>
     <t>Jupiter: Opponents hand gets shuffled and they can't see any of their cards</t>
+  </si>
+  <si>
+    <t>Veruna: can use a spell card free of cost</t>
+  </si>
+  <si>
+    <t>Karttikeyn: half of your creatures can attack again this turn</t>
+  </si>
+  <si>
+    <t>Rati: Can heal one of your creatures</t>
+  </si>
+  <si>
+    <t>Indra: able to look at a persons hand</t>
+  </si>
+  <si>
+    <t>Yama: either take the top card from your discard pile or your opponents</t>
+  </si>
+  <si>
+    <t>Agni: Draw an extra card or two</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -539,13 +539,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -553,13 +553,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -567,13 +567,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -581,13 +581,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -595,13 +595,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -609,19 +609,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -631,65 +628,68 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>